<commit_message>
feat: add dataset management
</commit_message>
<xml_diff>
--- a/dataset/pdf_list.xlsx
+++ b/dataset/pdf_list.xlsx
@@ -14,12 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>filename</t>
   </si>
   <si>
+    <t>filetype</t>
+  </si>
+  <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>&lt;function uuid4 at 0x00000139252036A0&gt;</t>
   </si>
   <si>
     <t>Beasiswa.pdf</t>
@@ -89,14 +104,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -113,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,23 +159,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,14 +492,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="60.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="29.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -473,173 +513,353 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2024</v>
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F2" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2024</v>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F3" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2024</v>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F4" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2024</v>
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F5" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2024</v>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F6" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2024</v>
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F7" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2024</v>
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F8" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2024</v>
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F9" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2024</v>
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F10" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2024</v>
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F11" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2024</v>
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F12" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2024</v>
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F13" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2024</v>
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F14" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2024</v>
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F15" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2019</v>
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F16" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="3">
-        <v>2021</v>
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F17" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2024</v>
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F18" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2017</v>
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F19" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2024</v>
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F20" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2024</v>
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F21" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2024</v>
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4">
+        <v>25569.333861898147</v>
+      </c>
+      <c r="F22" s="4">
+        <v>25569.333861898147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>